<commit_message>
optimize and fix some bug
add upload update on user ppic
</commit_message>
<xml_diff>
--- a/public/sj.xlsx
+++ b/public/sj.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\xampp7\htdocs\sj\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\satria-eko\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA61F78-316B-4415-9949-EB58F85E6031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>CYCLE</t>
   </si>
@@ -51,12 +52,78 @@
   </si>
   <si>
     <t>19J922000008242</t>
+  </si>
+  <si>
+    <t>19J922000008241</t>
+  </si>
+  <si>
+    <t>7A00032</t>
+  </si>
+  <si>
+    <t>SJA/19/998152</t>
+  </si>
+  <si>
+    <t>7A00033</t>
+  </si>
+  <si>
+    <t>SJA/19/998153</t>
+  </si>
+  <si>
+    <t>19J922000008243</t>
+  </si>
+  <si>
+    <t>SJA/19/998154</t>
+  </si>
+  <si>
+    <t>19J922000008244</t>
+  </si>
+  <si>
+    <t>7A00035</t>
+  </si>
+  <si>
+    <t>SJA/19/998155</t>
+  </si>
+  <si>
+    <t>19J922000008245</t>
+  </si>
+  <si>
+    <t>7A00036</t>
+  </si>
+  <si>
+    <t>SJA/19/998156</t>
+  </si>
+  <si>
+    <t>19J922000008246</t>
+  </si>
+  <si>
+    <t>7A00037</t>
+  </si>
+  <si>
+    <t>19J922000008247</t>
+  </si>
+  <si>
+    <t>7A00038</t>
+  </si>
+  <si>
+    <t>SJA/19/998158</t>
+  </si>
+  <si>
+    <t>19J922000008248</t>
+  </si>
+  <si>
+    <t>7A00039</t>
+  </si>
+  <si>
+    <t>SJA/19/998159</t>
+  </si>
+  <si>
+    <t>19J922000008249</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,11 +471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +511,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <v>20190410</v>
+        <v>20220616</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -459,16 +526,168 @@
         <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6190015950</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6190015953</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6190015957</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6190015962</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6190015968</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6190015975</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6190015983</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>20220616</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6190015992</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>